<commit_message>
bug fix & add assets.
</commit_message>
<xml_diff>
--- a/Tools/Luban/Datas/Gears.xlsx
+++ b/Tools/Luban/Datas/Gears.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5F8B95-E883-42A8-90F9-272C16EB3CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59588C20-1BA1-44FF-8465-BBDCDA88341B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
     <sheet name="Bodies" sheetId="2" r:id="rId2"/>
     <sheet name="Shields" sheetId="3" r:id="rId3"/>
+    <sheet name="Todo" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>##var</t>
   </si>
@@ -109,14 +110,8 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Assault</t>
-  </si>
-  <si>
     <t>猎狗</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Courser</t>
   </si>
   <si>
     <t>加速度</t>
@@ -144,6 +139,33 @@
   </si>
   <si>
     <t>float</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Courser</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assault</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>发射武器时机动性降低</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击时，8% 的几率强化子弹
+武器射速、武器扩散和射弹速度提高 15%
++15% 对攻击时降低移速的抵抗力
+- 10% 最大护盾</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>+3 子弹数量
++10% 武器射速
+-60% 武器扩散
+你的武器从两门舷侧加农炮发射，你的射弹将在它们之间分开
+-10% 武器伤害、爆炸半径和射弹尺寸</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3156,8 +3178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67386E97-BB97-4EB7-8CDE-19B42E092934}">
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -3165,7 +3187,7 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" style="9" customWidth="1"/>
     <col min="5" max="5" width="14" style="9" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" style="9" customWidth="1"/>
     <col min="7" max="7" width="18" style="9" customWidth="1"/>
@@ -3198,13 +3220,13 @@
         <v>17</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -3239,13 +3261,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -3307,13 +3329,13 @@
         <v>18</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -3331,7 +3353,7 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
     </row>
-    <row r="5" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" ht="73.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <v>1001</v>
@@ -3340,10 +3362,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4">
         <v>1000</v>
@@ -3370,19 +3392,19 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23" ht="108.95" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>1002</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4">
         <v>1400</v>
@@ -5776,4 +5798,25 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096A6ACB-0881-400A-98F3-58ECCC987496}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some qol and bug fix
</commit_message>
<xml_diff>
--- a/Tools/Luban/Datas/Gears.xlsx
+++ b/Tools/Luban/Datas/Gears.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC4C1F6-2B27-445C-9F69-D7701B801C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629BB394-5302-4D0C-A358-C1274A48E0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -142,14 +142,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>+3 子弹数量
-+10% 武器射速
--60% 武器扩散
-你的武器从两门舷侧加农炮发射，你的射弹将在它们之间分开
--10% 武器伤害、爆炸半径和射弹尺寸</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>默认武器</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -394,23 +386,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>受到伤害时额外发射一枚子弹
-+5 %伤害</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1,0.05</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Breaker</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击时，8% 的几率强化子弹
-武器射速、武器扩散和射弹速度提高 15%
-- 60% 射击减速度
-- 10% 最大护盾</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -457,6 +437,29 @@
     <t>射击子弹为圆形
 射击时子弹数量 +3
 子弹寿命 -50%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击时，8% 的几率强化子弹
+武器射速、武器扩散和射弹速度提高 15%
+- 60% 射击减速度
+- 10% 最大护盾
+适中的速度与略低的血量</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>+3 子弹数量
++10% 武器射速
+-60% 武器扩散
+你的武器从两门舷侧加农炮发射，你的射弹将在它们之间分开
+-10% 武器伤害、爆炸半径和射弹尺寸
+较高的速度与较低的血量</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>受到伤害时额外发射一枚子弹
++5 %伤害
+适中的速度与适中的血量</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -932,10 +935,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -977,10 +980,10 @@
         <v>12</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -1082,10 +1085,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -1110,13 +1113,13 @@
         <v>1000</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>29</v>
-      </c>
       <c r="E5" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="21">
         <v>0</v>
@@ -1147,13 +1150,13 @@
         <v>1001</v>
       </c>
       <c r="C6" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="21" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>46</v>
       </c>
       <c r="F6" s="21">
         <v>0</v>
@@ -1184,13 +1187,13 @@
         <v>1002</v>
       </c>
       <c r="C7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>72</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>73</v>
       </c>
       <c r="F7" s="21">
         <v>0</v>
@@ -1221,13 +1224,13 @@
         <v>1003</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -1260,13 +1263,13 @@
         <v>1001</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F9" s="21">
         <v>0</v>
@@ -1302,7 +1305,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>14</v>
@@ -3516,8 +3519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67386E97-BB97-4EB7-8CDE-19B42E092934}">
   <dimension ref="A1:Y101"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -3556,16 +3559,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>21</v>
@@ -3603,7 +3606,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>23</v>
@@ -3679,16 +3682,16 @@
         <v>10</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>19</v>
@@ -3718,20 +3721,20 @@
         <v>1000</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20">
         <v>100</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="21">
         <v>1000</v>
@@ -3755,7 +3758,7 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
     </row>
-    <row r="6" spans="1:25" ht="73.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25" ht="91.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="19"/>
       <c r="B6" s="19">
         <v>1001</v>
@@ -3764,13 +3767,13 @@
         <v>15</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="20">
         <v>90</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="20">
-        <v>100</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>25</v>
@@ -3800,7 +3803,7 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
     </row>
-    <row r="7" spans="1:25" ht="95.6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25" ht="111.35" x14ac:dyDescent="0.45">
       <c r="A7" s="19"/>
       <c r="B7" s="19">
         <v>1002</v>
@@ -3809,13 +3812,13 @@
         <v>18</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="20">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>24</v>
@@ -3827,7 +3830,7 @@
         <v>1400</v>
       </c>
       <c r="J7" s="21">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -3853,22 +3856,22 @@
         <v>1234</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>84</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>85</v>
       </c>
       <c r="F8" s="20">
         <v>100</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I8" s="21">
         <v>1400</v>
@@ -3892,34 +3895,34 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
     </row>
-    <row r="9" spans="1:25" ht="36.299999999999997" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25" ht="54.45" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>1003</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="F9" s="20">
         <v>100</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I9" s="21">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="J9" s="21">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -6458,13 +6461,13 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>12</v>
@@ -6519,7 +6522,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>23</v>
@@ -6628,10 +6631,10 @@
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>13</v>
@@ -6678,22 +6681,22 @@
         <v>1000</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -6737,22 +6740,22 @@
         <v>1001</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -6796,22 +6799,22 @@
         <v>1002</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="F7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -6855,22 +6858,22 @@
         <v>1003</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="F8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -6914,13 +6917,13 @@
         <v>1004</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>80</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>81</v>
       </c>
       <c r="F9" s="20">
         <v>100</v>
@@ -6929,7 +6932,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
@@ -6975,13 +6978,13 @@
         <v>1004</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>78</v>
-      </c>
       <c r="E10" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>

</xml_diff>